<commit_message>
Added table/figure descriptions Added Analysis chapter
</commit_message>
<xml_diff>
--- a/Praca dyplomowa, wyniki.xlsx
+++ b/Praca dyplomowa, wyniki.xlsx
@@ -17,7 +17,8 @@
     <sheet name="CF mm" sheetId="4" r:id="rId3"/>
     <sheet name="Fake CF ab" sheetId="6" r:id="rId4"/>
     <sheet name="CF real AB" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId6"/>
+    <sheet name="TTT real AB" sheetId="8" r:id="rId6"/>
+    <sheet name="TTT CvC" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="17">
   <si>
     <t>Iteration</t>
   </si>
@@ -75,15 +76,22 @@
   <si>
     <t>Time/Checks</t>
   </si>
+  <si>
+    <t>Player 1</t>
+  </si>
+  <si>
+    <t>Player 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -115,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -123,6 +131,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1079,36 +1090,36 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'TTT mm'!$E$5:$E$13</c:f>
+              <c:f>'TTT mm'!$J$29:$J$37</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2179.2314190000002</c:v>
+                  <c:v>1245.0068430000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73.934687999999994</c:v>
+                  <c:v>43.328568999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.41568</c:v>
+                  <c:v>3.368706</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.37105500000000002</c:v>
+                  <c:v>0.43118699999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10302699999999999</c:v>
+                  <c:v>0.103948</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.4211E-2</c:v>
+                  <c:v>4.1842333333333336E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8948E-2</c:v>
+                  <c:v>1.8553E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1447000000000001E-2</c:v>
+                  <c:v>1.3289666666666667E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0264000000000001E-2</c:v>
+                  <c:v>9.3423333333333327E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1160,36 +1171,36 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'TTT mm'!$F$5:$F$13</c:f>
+              <c:f>'TTT mm'!$K$29:$K$37</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>57.114446999999998</c:v>
+                  <c:v>42.622642999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5013380000000001</c:v>
+                  <c:v>4.3709490000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58697699999999997</c:v>
+                  <c:v>0.442108</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.921E-2</c:v>
+                  <c:v>3.6184000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.1050000000000002E-3</c:v>
+                  <c:v>6.8420000000000009E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.5530000000000002E-3</c:v>
+                  <c:v>3.2896666666666669E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9729999999999999E-3</c:v>
+                  <c:v>2.2366666666666668E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5790000000000001E-3</c:v>
+                  <c:v>1.7103333333333335E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.1839999999999999E-3</c:v>
+                  <c:v>1.4473333333333335E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1241,36 +1252,36 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'TTT mm'!$G$5:$G$13</c:f>
+              <c:f>'TTT mm'!$L$29:$L$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2236.3458660000001</c:v>
+                  <c:v>1287.629486</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77.436025999999998</c:v>
+                  <c:v>47.699517999999991</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0026570000000001</c:v>
+                  <c:v>3.8108140000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.40026500000000004</c:v>
+                  <c:v>0.46737099999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11013199999999999</c:v>
+                  <c:v>0.11079</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.7764000000000001E-2</c:v>
+                  <c:v>4.5132000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0920999999999999E-2</c:v>
+                  <c:v>2.0789666666666668E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3026000000000001E-2</c:v>
+                  <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.1448E-2</c:v>
+                  <c:v>1.0789666666666668E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1381,7 +1392,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3190,6 +3201,404 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Time to check each move</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CF real AB'!$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time/Checks</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'CF real AB'!$D$5:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>16910</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8636</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19236</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28285</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20441</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11570</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24091</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23305</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18482</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23580</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16028</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19469</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11880</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5128</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>915</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'CF real AB'!$G$5:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.7667180366646952E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8605766558591941E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1178213765855687E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2955720700017679E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4444460153612837E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4966201382886778E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.4704188286081942E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0360570692984336E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2087282761605886E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1819068702290077E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0513276765660095E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0243506600236274E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.6602634680134681E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3564857644305772E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5472612021857923E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-15CF-4BC4-B717-A18416B42687}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="216674872"/>
+        <c:axId val="216674216"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="216674872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="216674216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="216674216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="216674872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3430,6 +3839,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -5946,6 +6395,509 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6530,15 +7482,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>328612</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>366712</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>61912</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6675,6 +7627,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33B6CC61-54B9-4096-A02A-BF057CF78BF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6982,7 +7975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
@@ -7959,12 +8952,16 @@
   <dimension ref="B2:R41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
@@ -8211,7 +9208,7 @@
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="R14" s="3"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>0</v>
       </c>
@@ -8231,14 +9228,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19">
         <v>9</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="6">
         <v>255168</v>
       </c>
       <c r="E19">
@@ -8255,14 +9252,14 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20">
         <v>9</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="6">
         <v>27732</v>
       </c>
       <c r="E20">
@@ -8279,14 +9276,14 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>3</v>
       </c>
       <c r="C21">
         <v>9</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="6">
         <v>3468</v>
       </c>
       <c r="E21">
@@ -8303,14 +9300,14 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>4</v>
       </c>
       <c r="C22">
         <v>9</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="6">
         <v>457</v>
       </c>
       <c r="E22">
@@ -8327,14 +9324,14 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>5</v>
       </c>
       <c r="C23">
         <v>9</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="6">
         <v>94</v>
       </c>
       <c r="E23">
@@ -8351,14 +9348,14 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>6</v>
       </c>
       <c r="C24">
         <v>9</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="6">
         <v>21</v>
       </c>
       <c r="E24">
@@ -8375,14 +9372,14 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>7</v>
       </c>
       <c r="C25">
         <v>9</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="6">
         <v>6</v>
       </c>
       <c r="E25">
@@ -8399,14 +9396,14 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>8</v>
       </c>
       <c r="C26">
         <v>9</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="6">
         <v>2</v>
       </c>
       <c r="E26">
@@ -8423,14 +9420,14 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>9</v>
       </c>
       <c r="C27">
         <v>9</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="6">
         <v>1</v>
       </c>
       <c r="E27">
@@ -8447,7 +9444,61 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J29" s="1">
+        <f t="shared" ref="J29:K36" si="2">(E5+E19+E33)/3</f>
+        <v>1245.0068430000001</v>
+      </c>
+      <c r="K29" s="1">
+        <f t="shared" si="2"/>
+        <v>42.622642999999997</v>
+      </c>
+      <c r="L29" s="1">
+        <f>(G5+G19+G33)/3</f>
+        <v>1287.629486</v>
+      </c>
+      <c r="M29" s="1">
+        <f>L29/D19</f>
+        <v>5.0462028389139709E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J30" s="1">
+        <f t="shared" si="2"/>
+        <v>43.328568999999995</v>
+      </c>
+      <c r="K30" s="1">
+        <f t="shared" si="2"/>
+        <v>4.3709490000000004</v>
+      </c>
+      <c r="L30" s="1">
+        <f t="shared" ref="L30:L36" si="3">(G6+G20+G34)/3</f>
+        <v>47.699517999999991</v>
+      </c>
+      <c r="M30" s="1">
+        <f t="shared" ref="M30:M36" si="4">L30/D20</f>
+        <v>1.7200172364055962E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J31" s="1">
+        <f t="shared" si="2"/>
+        <v>3.368706</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" si="2"/>
+        <v>0.442108</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="3"/>
+        <v>3.8108140000000001</v>
+      </c>
+      <c r="M31" s="1">
+        <f t="shared" si="4"/>
+        <v>1.0988506343713956E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>0</v>
       </c>
@@ -8466,8 +9517,24 @@
       <c r="G32" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J32" s="1">
+        <f t="shared" si="2"/>
+        <v>0.43118699999999999</v>
+      </c>
+      <c r="K32" s="1">
+        <f t="shared" si="2"/>
+        <v>3.6184000000000001E-2</v>
+      </c>
+      <c r="L32" s="1">
+        <f t="shared" si="3"/>
+        <v>0.46737099999999998</v>
+      </c>
+      <c r="M32" s="1">
+        <f t="shared" si="4"/>
+        <v>1.0226936542669584E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>1</v>
       </c>
@@ -8489,9 +9556,24 @@
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J33" s="1">
+        <f t="shared" si="2"/>
+        <v>0.103948</v>
+      </c>
+      <c r="K33" s="1">
+        <f t="shared" si="2"/>
+        <v>6.8420000000000009E-3</v>
+      </c>
+      <c r="L33" s="1">
+        <f t="shared" si="3"/>
+        <v>0.11079</v>
+      </c>
+      <c r="M33" s="1">
+        <f t="shared" si="4"/>
+        <v>1.1786170212765958E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>2</v>
       </c>
@@ -8508,14 +9590,29 @@
         <v>4.5762140000000002</v>
       </c>
       <c r="G34" s="1">
-        <f t="shared" ref="G34:G41" si="2">E34+F34</f>
+        <f t="shared" ref="G34:G41" si="5">E34+F34</f>
         <v>32.738894999999999</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J34" s="1">
+        <f t="shared" si="2"/>
+        <v>4.1842333333333336E-2</v>
+      </c>
+      <c r="K34" s="1">
+        <f t="shared" si="2"/>
+        <v>3.2896666666666669E-3</v>
+      </c>
+      <c r="L34" s="1">
+        <f t="shared" si="3"/>
+        <v>4.5132000000000005E-2</v>
+      </c>
+      <c r="M34" s="1">
+        <f t="shared" si="4"/>
+        <v>2.1491428571428573E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>3</v>
       </c>
@@ -8532,14 +9629,29 @@
         <v>0.375002</v>
       </c>
       <c r="G35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3.6296279999999999</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J35" s="1">
+        <f t="shared" si="2"/>
+        <v>1.8553E-2</v>
+      </c>
+      <c r="K35" s="1">
+        <f t="shared" si="2"/>
+        <v>2.2366666666666668E-3</v>
+      </c>
+      <c r="L35" s="1">
+        <f t="shared" si="3"/>
+        <v>2.0789666666666668E-2</v>
+      </c>
+      <c r="M35" s="1">
+        <f t="shared" si="4"/>
+        <v>3.4649444444444445E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>4</v>
       </c>
@@ -8556,14 +9668,29 @@
         <v>4.3421000000000001E-2</v>
       </c>
       <c r="G36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.46894999999999998</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J36" s="1">
+        <f t="shared" si="2"/>
+        <v>1.3289666666666667E-2</v>
+      </c>
+      <c r="K36" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7103333333333335E-3</v>
+      </c>
+      <c r="L36" s="1">
+        <f t="shared" si="3"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M36" s="1">
+        <f t="shared" si="4"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>5</v>
       </c>
@@ -8580,14 +9707,29 @@
         <v>6.3160000000000004E-3</v>
       </c>
       <c r="G37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.108158</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J37" s="1">
+        <f t="shared" ref="J37:K37" si="6">(E13+E27+E41)/3</f>
+        <v>9.3423333333333327E-3</v>
+      </c>
+      <c r="K37" s="1">
+        <f t="shared" si="6"/>
+        <v>1.4473333333333335E-3</v>
+      </c>
+      <c r="L37" s="1">
+        <f>(G13+G27+G41)/3</f>
+        <v>1.0789666666666668E-2</v>
+      </c>
+      <c r="M37" s="1">
+        <f>L37/D27</f>
+        <v>1.0789666666666668E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>6</v>
       </c>
@@ -8604,14 +9746,15 @@
         <v>3.5530000000000002E-3</v>
       </c>
       <c r="G38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5.2106E-2</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L38" s="8"/>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>7</v>
       </c>
@@ -8628,14 +9771,14 @@
         <v>1.9740000000000001E-3</v>
       </c>
       <c r="G39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.9737000000000001E-2</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>8</v>
       </c>
@@ -8652,14 +9795,14 @@
         <v>1.5790000000000001E-3</v>
       </c>
       <c r="G40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.3027E-2</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>9</v>
       </c>
@@ -8676,7 +9819,7 @@
         <v>1.9740000000000001E-3</v>
       </c>
       <c r="G41" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.0658000000000001E-2</v>
       </c>
       <c r="H41" s="1"/>
@@ -8694,8 +9837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC97"/>
   <sheetViews>
-    <sheetView topLeftCell="D14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12335,18 +13478,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:V21"/>
+  <dimension ref="C4:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y5" sqref="Y5"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>4</v>
       </c>
@@ -12363,11 +13509,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>7</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <v>16910</v>
       </c>
       <c r="E5" s="6">
@@ -12381,11 +13527,11 @@
         <v>2.7667180366646952E-3</v>
       </c>
     </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>7</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="7">
         <v>8636</v>
       </c>
       <c r="E6" s="6">
@@ -12399,11 +13545,11 @@
         <v>1.8605766558591941E-3</v>
       </c>
     </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>7</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="7">
         <v>19236</v>
       </c>
       <c r="E7" s="6">
@@ -12416,30 +13562,12 @@
         <f t="shared" si="0"/>
         <v>1.1178213765855687E-3</v>
       </c>
-      <c r="Q7" t="s">
-        <v>11</v>
-      </c>
-      <c r="R7">
-        <v>7</v>
-      </c>
-      <c r="S7">
-        <v>16910</v>
-      </c>
-      <c r="T7">
-        <v>4271</v>
-      </c>
-      <c r="U7">
-        <v>0.73064099999999998</v>
-      </c>
-      <c r="V7">
-        <v>46.785201999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>7</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="7">
         <v>28285</v>
       </c>
       <c r="E8" s="6">
@@ -12452,30 +13580,12 @@
         <f t="shared" si="0"/>
         <v>1.2955720700017679E-3</v>
       </c>
-      <c r="Q8" t="s">
-        <v>11</v>
-      </c>
-      <c r="R8">
-        <v>7</v>
-      </c>
-      <c r="S8">
-        <v>8636</v>
-      </c>
-      <c r="T8">
-        <v>1378</v>
-      </c>
-      <c r="U8">
-        <v>2.8709999999999999E-3</v>
-      </c>
-      <c r="V8">
-        <v>16.06794</v>
-      </c>
-    </row>
-    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>7</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="7">
         <v>20441</v>
       </c>
       <c r="E9" s="6">
@@ -12488,30 +13598,12 @@
         <f t="shared" si="0"/>
         <v>1.4444460153612837E-3</v>
       </c>
-      <c r="Q9" t="s">
-        <v>11</v>
-      </c>
-      <c r="R9">
-        <v>7</v>
-      </c>
-      <c r="S9">
-        <v>19236</v>
-      </c>
-      <c r="T9">
-        <v>5216</v>
-      </c>
-      <c r="U9">
-        <v>1.6410000000000001E-3</v>
-      </c>
-      <c r="V9">
-        <v>21.502412</v>
-      </c>
-    </row>
-    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>7</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="7">
         <v>11570</v>
       </c>
       <c r="E10" s="6">
@@ -12524,30 +13616,12 @@
         <f t="shared" si="0"/>
         <v>1.4966201382886778E-3</v>
       </c>
-      <c r="Q10" t="s">
-        <v>11</v>
-      </c>
-      <c r="R10">
-        <v>7</v>
-      </c>
-      <c r="S10">
-        <v>28285</v>
-      </c>
-      <c r="T10">
-        <v>8481</v>
-      </c>
-      <c r="U10">
-        <v>3.2820000000000002E-3</v>
-      </c>
-      <c r="V10">
-        <v>36.645256000000003</v>
-      </c>
-    </row>
-    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>7</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="7">
         <v>24091</v>
       </c>
       <c r="E11" s="6">
@@ -12560,30 +13634,12 @@
         <f t="shared" si="0"/>
         <v>9.4704188286081942E-4</v>
       </c>
-      <c r="Q11" t="s">
-        <v>11</v>
-      </c>
-      <c r="R11">
-        <v>7</v>
-      </c>
-      <c r="S11">
-        <v>20441</v>
-      </c>
-      <c r="T11">
-        <v>5457</v>
-      </c>
-      <c r="U11">
-        <v>2.872E-3</v>
-      </c>
-      <c r="V11">
-        <v>29.525921</v>
-      </c>
-    </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>7</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="7">
         <v>23305</v>
       </c>
       <c r="E12" s="6">
@@ -12596,30 +13652,12 @@
         <f t="shared" si="0"/>
         <v>9.0360570692984336E-4</v>
       </c>
-      <c r="Q12" t="s">
-        <v>11</v>
-      </c>
-      <c r="R12">
-        <v>7</v>
-      </c>
-      <c r="S12">
-        <v>11570</v>
-      </c>
-      <c r="T12">
-        <v>2140</v>
-      </c>
-      <c r="U12">
-        <v>4.9230000000000003E-3</v>
-      </c>
-      <c r="V12">
-        <v>17.315895000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>7</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="7">
         <v>18482</v>
       </c>
       <c r="E13" s="6">
@@ -12632,30 +13670,12 @@
         <f t="shared" si="0"/>
         <v>1.2087282761605886E-3</v>
       </c>
-      <c r="Q13" t="s">
-        <v>11</v>
-      </c>
-      <c r="R13">
-        <v>7</v>
-      </c>
-      <c r="S13">
-        <v>24091</v>
-      </c>
-      <c r="T13">
-        <v>6119</v>
-      </c>
-      <c r="U13">
-        <v>1.6410000000000001E-3</v>
-      </c>
-      <c r="V13">
-        <v>22.815186000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>7</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="7">
         <v>23580</v>
       </c>
       <c r="E14" s="6">
@@ -12668,30 +13688,12 @@
         <f t="shared" si="0"/>
         <v>1.1819068702290077E-3</v>
       </c>
-      <c r="Q14" t="s">
-        <v>11</v>
-      </c>
-      <c r="R14">
-        <v>7</v>
-      </c>
-      <c r="S14">
-        <v>23305</v>
-      </c>
-      <c r="T14">
-        <v>6062</v>
-      </c>
-      <c r="U14">
-        <v>1.2310000000000001E-3</v>
-      </c>
-      <c r="V14">
-        <v>21.058530999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>7</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="7">
         <v>16028</v>
       </c>
       <c r="E15" s="6">
@@ -12704,30 +13706,12 @@
         <f t="shared" si="0"/>
         <v>1.0513276765660095E-3</v>
       </c>
-      <c r="Q15" t="s">
-        <v>11</v>
-      </c>
-      <c r="R15">
-        <v>7</v>
-      </c>
-      <c r="S15">
-        <v>18482</v>
-      </c>
-      <c r="T15">
-        <v>3875</v>
-      </c>
-      <c r="U15">
-        <v>1.6410000000000001E-3</v>
-      </c>
-      <c r="V15">
-        <v>22.339715999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>7</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="7">
         <v>19469</v>
       </c>
       <c r="E16" s="6">
@@ -12740,30 +13724,12 @@
         <f t="shared" si="0"/>
         <v>1.0243506600236274E-3</v>
       </c>
-      <c r="Q16" t="s">
-        <v>11</v>
-      </c>
-      <c r="R16">
-        <v>7</v>
-      </c>
-      <c r="S16">
-        <v>23580</v>
-      </c>
-      <c r="T16">
-        <v>5500</v>
-      </c>
-      <c r="U16">
-        <v>1.2310000000000001E-3</v>
-      </c>
-      <c r="V16">
-        <v>27.869364000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>7</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="7">
         <v>11880</v>
       </c>
       <c r="E17" s="6">
@@ -12776,30 +13742,12 @@
         <f t="shared" si="0"/>
         <v>7.6602634680134681E-4</v>
       </c>
-      <c r="Q17" t="s">
-        <v>11</v>
-      </c>
-      <c r="R17">
-        <v>7</v>
-      </c>
-      <c r="S17">
-        <v>16028</v>
-      </c>
-      <c r="T17">
-        <v>3326</v>
-      </c>
-      <c r="U17">
-        <v>2.4620000000000002E-3</v>
-      </c>
-      <c r="V17">
-        <v>16.850680000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>7</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="7">
         <v>5128</v>
       </c>
       <c r="E18" s="6">
@@ -12812,30 +13760,12 @@
         <f t="shared" si="0"/>
         <v>1.3564857644305772E-3</v>
       </c>
-      <c r="Q18" t="s">
-        <v>11</v>
-      </c>
-      <c r="R18">
-        <v>7</v>
-      </c>
-      <c r="S18">
-        <v>19469</v>
-      </c>
-      <c r="T18">
-        <v>4588</v>
-      </c>
-      <c r="U18">
-        <v>2.4620000000000002E-3</v>
-      </c>
-      <c r="V18">
-        <v>19.943083000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>7</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="7">
         <v>915</v>
       </c>
       <c r="E19" s="6">
@@ -12848,234 +13778,967 @@
         <f t="shared" si="0"/>
         <v>1.5472612021857923E-3</v>
       </c>
-      <c r="Q19" t="s">
+    </row>
+    <row r="23" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24" s="6">
+        <v>982</v>
+      </c>
+      <c r="E24" s="6">
+        <v>149</v>
+      </c>
+      <c r="F24" s="9">
+        <v>6.9524780000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25" s="6">
+        <v>6984</v>
+      </c>
+      <c r="E25" s="6">
+        <v>2210</v>
+      </c>
+      <c r="F25" s="9">
+        <v>11.098038000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>7</v>
+      </c>
+      <c r="D26" s="6">
+        <v>13167</v>
+      </c>
+      <c r="E26" s="6">
+        <v>2540</v>
+      </c>
+      <c r="F26" s="9">
+        <v>14.237258000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27" s="6">
+        <v>13167</v>
+      </c>
+      <c r="E27" s="6">
+        <v>2540</v>
+      </c>
+      <c r="F27" s="9">
+        <v>22.371251999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28" s="6">
+        <v>123509</v>
+      </c>
+      <c r="E28" s="6">
+        <v>37496</v>
+      </c>
+      <c r="F28" s="9">
+        <v>147.10848799999999</v>
+      </c>
+    </row>
+    <row r="29" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>9</v>
+      </c>
+      <c r="D29" s="6">
+        <v>167564</v>
+      </c>
+      <c r="E29" s="6">
+        <v>39037</v>
+      </c>
+      <c r="F29" s="9">
+        <v>137.896771</v>
+      </c>
+    </row>
+    <row r="30" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30" s="6">
+        <v>952511</v>
+      </c>
+      <c r="E30" s="6">
+        <v>272730</v>
+      </c>
+      <c r="F30" s="9">
+        <v>887.15586299999995</v>
+      </c>
+    </row>
+    <row r="31" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C31">
         <v>11</v>
       </c>
-      <c r="R19">
+      <c r="D31" s="6">
+        <v>1849059</v>
+      </c>
+      <c r="E31" s="6">
+        <v>522285</v>
+      </c>
+      <c r="F31" s="9">
+        <v>1926.2385810000001</v>
+      </c>
+    </row>
+    <row r="32" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>12</v>
+      </c>
+      <c r="D32" s="6">
+        <v>16501759</v>
+      </c>
+      <c r="E32" s="6">
+        <v>4949789</v>
+      </c>
+      <c r="F32" s="9">
+        <v>13807.394973</v>
+      </c>
+      <c r="R32" t="s">
+        <v>11</v>
+      </c>
+      <c r="S32">
+        <v>5</v>
+      </c>
+      <c r="T32">
+        <v>982</v>
+      </c>
+      <c r="U32">
+        <v>149</v>
+      </c>
+      <c r="V32">
+        <v>1.133926</v>
+      </c>
+      <c r="W32">
+        <v>6.9524780000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>13</v>
+      </c>
+      <c r="D33" s="6">
+        <v>31786281</v>
+      </c>
+      <c r="E33" s="6">
+        <v>10805507</v>
+      </c>
+      <c r="F33" s="9">
+        <v>27591.887010999999</v>
+      </c>
+      <c r="R33" t="s">
+        <v>11</v>
+      </c>
+      <c r="S33">
+        <v>6</v>
+      </c>
+      <c r="T33">
+        <v>6984</v>
+      </c>
+      <c r="U33">
+        <v>2210</v>
+      </c>
+      <c r="V33">
+        <v>2.0509999999999999E-3</v>
+      </c>
+      <c r="W33">
+        <v>11.098038000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>14</v>
+      </c>
+      <c r="D34" s="6">
+        <v>335138373</v>
+      </c>
+      <c r="E34" s="6">
+        <v>101386483</v>
+      </c>
+      <c r="F34" s="9">
+        <v>285578.331175</v>
+      </c>
+      <c r="R34" t="s">
+        <v>11</v>
+      </c>
+      <c r="S34">
         <v>7</v>
       </c>
-      <c r="S19">
-        <v>11880</v>
-      </c>
-      <c r="T19">
-        <v>2853</v>
-      </c>
-      <c r="U19">
+      <c r="T34">
+        <v>13167</v>
+      </c>
+      <c r="U34">
+        <v>2540</v>
+      </c>
+      <c r="V34">
         <v>1.2310000000000001E-3</v>
       </c>
-      <c r="V19">
-        <v>9.1003930000000004</v>
-      </c>
-    </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="Q20" t="s">
+      <c r="W34">
+        <v>14.237258000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="R35" t="s">
         <v>11</v>
       </c>
-      <c r="R20">
+      <c r="S35">
         <v>7</v>
       </c>
-      <c r="S20">
-        <v>5128</v>
-      </c>
-      <c r="T20">
-        <v>1283</v>
-      </c>
-      <c r="U20">
-        <v>2.0509999999999999E-3</v>
-      </c>
-      <c r="V20">
-        <v>6.9560589999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="Q21" t="s">
+      <c r="T35">
+        <v>13167</v>
+      </c>
+      <c r="U35">
+        <v>2540</v>
+      </c>
+      <c r="V35">
+        <v>1.2310000000000001E-3</v>
+      </c>
+      <c r="W35">
+        <v>22.371251999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="R36" t="s">
         <v>11</v>
       </c>
-      <c r="R21">
-        <v>7</v>
-      </c>
-      <c r="S21">
-        <v>915</v>
-      </c>
-      <c r="T21">
-        <v>257</v>
-      </c>
-      <c r="U21">
+      <c r="S36">
+        <v>8</v>
+      </c>
+      <c r="T36">
+        <v>123509</v>
+      </c>
+      <c r="U36">
+        <v>37496</v>
+      </c>
+      <c r="V36">
         <v>1.6410000000000001E-3</v>
       </c>
-      <c r="V21">
-        <v>1.4157439999999999</v>
+      <c r="W36">
+        <v>147.10848799999999</v>
+      </c>
+    </row>
+    <row r="37" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="R37" t="s">
+        <v>11</v>
+      </c>
+      <c r="S37">
+        <v>9</v>
+      </c>
+      <c r="T37">
+        <v>167564</v>
+      </c>
+      <c r="U37">
+        <v>39037</v>
+      </c>
+      <c r="V37">
+        <v>1.6410000000000001E-3</v>
+      </c>
+      <c r="W37">
+        <v>137.896771</v>
+      </c>
+    </row>
+    <row r="38" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="R38" t="s">
+        <v>11</v>
+      </c>
+      <c r="S38">
+        <v>10</v>
+      </c>
+      <c r="T38">
+        <v>952511</v>
+      </c>
+      <c r="U38">
+        <v>272730</v>
+      </c>
+      <c r="V38">
+        <v>1.6410000000000001E-3</v>
+      </c>
+      <c r="W38">
+        <v>887.15586299999995</v>
+      </c>
+    </row>
+    <row r="39" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="R39" t="s">
+        <v>11</v>
+      </c>
+      <c r="S39">
+        <v>11</v>
+      </c>
+      <c r="T39">
+        <v>1849059</v>
+      </c>
+      <c r="U39">
+        <v>522285</v>
+      </c>
+      <c r="V39">
+        <v>1.2310000000000001E-3</v>
+      </c>
+      <c r="W39">
+        <v>1926.2385810000001</v>
+      </c>
+    </row>
+    <row r="40" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="R40" t="s">
+        <v>11</v>
+      </c>
+      <c r="S40">
+        <v>12</v>
+      </c>
+      <c r="T40">
+        <v>16501759</v>
+      </c>
+      <c r="U40">
+        <v>4949789</v>
+      </c>
+      <c r="V40">
+        <v>1.23E-3</v>
+      </c>
+      <c r="W40">
+        <v>13807.394973</v>
+      </c>
+    </row>
+    <row r="41" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="R41" t="s">
+        <v>11</v>
+      </c>
+      <c r="S41">
+        <v>13</v>
+      </c>
+      <c r="T41">
+        <v>31786281</v>
+      </c>
+      <c r="U41">
+        <v>10805507</v>
+      </c>
+      <c r="V41">
+        <v>1.6410000000000001E-3</v>
+      </c>
+      <c r="W41">
+        <v>27591.887010999999</v>
+      </c>
+    </row>
+    <row r="42" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="R42" t="s">
+        <v>11</v>
+      </c>
+      <c r="S42">
+        <v>14</v>
+      </c>
+      <c r="T42">
+        <v>335138373</v>
+      </c>
+      <c r="U42">
+        <v>101386483</v>
+      </c>
+      <c r="V42">
+        <v>1.6410000000000001E-3</v>
+      </c>
+      <c r="W42">
+        <v>285578.331175</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="N15:T23"/>
+  <dimension ref="C4:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T16" sqref="T16:T18"/>
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>13373</v>
+      </c>
+      <c r="E5">
+        <v>5750</v>
+      </c>
+      <c r="F5">
+        <v>7.7768569999999997</v>
+      </c>
+      <c r="G5" s="1">
+        <f>F5/D5</f>
+        <v>5.8153421072309878E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>965</v>
+      </c>
+      <c r="E6">
+        <v>482</v>
+      </c>
+      <c r="F6">
+        <v>0.72119599999999995</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" ref="G6:G13" si="0">F6/D6</f>
+        <v>7.4735336787564767E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>38</v>
+      </c>
+      <c r="E7">
+        <v>19</v>
+      </c>
+      <c r="F7">
+        <v>2.6665000000000001E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>7.0171052631578948E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>75</v>
+      </c>
+      <c r="E8">
+        <v>37</v>
+      </c>
+      <c r="F8">
+        <v>6.2766000000000002E-2</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>8.3688000000000002E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>64</v>
+      </c>
+      <c r="E9">
+        <v>32</v>
+      </c>
+      <c r="F9">
+        <v>4.9228000000000001E-2</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>7.6918750000000001E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>2.0923000000000001E-2</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>8.3692E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>2.4614E-2</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="0"/>
+        <v>4.1023333333333337E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>5.3330000000000001E-3</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0666E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>6.1539999999999997E-3</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>3.0769999999999999E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="7"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="7"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D16" s="7"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D17" s="7"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="7"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D19" s="7"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="15" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N15" t="s">
-        <v>10</v>
-      </c>
-      <c r="O15">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
         <v>7</v>
       </c>
-      <c r="P15">
-        <v>823536</v>
-      </c>
-      <c r="Q15">
-        <v>5020.449732</v>
-      </c>
-      <c r="R15">
-        <v>55.799854000000003</v>
-      </c>
-      <c r="T15">
-        <f>R15/R20</f>
-        <v>8.9999996774185238</v>
-      </c>
-    </row>
-    <row r="16" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N16" t="s">
-        <v>10</v>
-      </c>
-      <c r="O16">
+      <c r="K3">
+        <v>8</v>
+      </c>
+      <c r="L3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>-1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>-1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>-1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C10">
         <v>7</v>
       </c>
-      <c r="P16">
-        <v>823494</v>
-      </c>
-      <c r="Q16">
-        <v>2630.6937969999999</v>
-      </c>
-      <c r="R16">
-        <v>41.095968999999997</v>
-      </c>
-      <c r="T16">
-        <f t="shared" ref="T16:T18" si="0">R16/R21</f>
-        <v>12.32316147983601</v>
-      </c>
-    </row>
-    <row r="17" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N17" t="s">
-        <v>10</v>
-      </c>
-      <c r="O17">
-        <v>7</v>
-      </c>
-      <c r="P17">
-        <v>822738</v>
-      </c>
-      <c r="Q17">
-        <v>2947.450081</v>
-      </c>
-      <c r="R17">
-        <v>41.298217999999999</v>
-      </c>
-      <c r="T17">
-        <f t="shared" si="0"/>
-        <v>14.698203325140421</v>
-      </c>
-    </row>
-    <row r="18" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N18" t="s">
-        <v>10</v>
-      </c>
-      <c r="O18">
-        <v>7</v>
-      </c>
-      <c r="P18">
-        <v>822696</v>
-      </c>
-      <c r="Q18">
-        <v>1767.2349750000001</v>
-      </c>
-      <c r="R18">
-        <v>41.002844000000003</v>
-      </c>
-      <c r="T18">
-        <f t="shared" si="0"/>
-        <v>14.924295030663659</v>
-      </c>
-    </row>
-    <row r="20" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N20" t="s">
-        <v>10</v>
-      </c>
-      <c r="O20">
-        <v>7</v>
-      </c>
-      <c r="P20">
-        <v>823536</v>
-      </c>
-      <c r="Q20">
-        <v>4475.4722599999996</v>
-      </c>
-      <c r="R20">
-        <v>6.1999839999999997</v>
-      </c>
-    </row>
-    <row r="21" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N21" t="s">
-        <v>10</v>
-      </c>
-      <c r="O21">
-        <v>7</v>
-      </c>
-      <c r="P21">
-        <v>823494</v>
-      </c>
-      <c r="Q21">
-        <v>2344.0271050000001</v>
-      </c>
-      <c r="R21">
-        <v>3.3348559999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N22" t="s">
-        <v>10</v>
-      </c>
-      <c r="O22">
-        <v>7</v>
-      </c>
-      <c r="P22">
-        <v>822738</v>
-      </c>
-      <c r="Q22">
-        <v>2713.3681790000001</v>
-      </c>
-      <c r="R22">
-        <v>2.8097460000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N23" t="s">
-        <v>10</v>
-      </c>
-      <c r="O23">
-        <v>7</v>
-      </c>
-      <c r="P23">
-        <v>822696</v>
-      </c>
-      <c r="Q23">
-        <v>2057.7037869999999</v>
-      </c>
-      <c r="R23">
-        <v>2.7473890000000001</v>
+      <c r="D10">
+        <v>-1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>-1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Wersja wysylana do promotora Poprawki formatowania, rozwiniecie rozdzialu Analizy
</commit_message>
<xml_diff>
--- a/Praca dyplomowa, wyniki.xlsx
+++ b/Praca dyplomowa, wyniki.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24525" windowHeight="12210" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24525" windowHeight="12210" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="TTT ab 1" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,10 @@
     <sheet name="CF mm" sheetId="4" r:id="rId3"/>
     <sheet name="Fake CF ab" sheetId="6" r:id="rId4"/>
     <sheet name="CF real AB" sheetId="7" r:id="rId5"/>
-    <sheet name="TTT real AB" sheetId="8" r:id="rId6"/>
-    <sheet name="TTT CvC" sheetId="5" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId6"/>
+    <sheet name="TTT real AB" sheetId="8" r:id="rId7"/>
+    <sheet name="TTT CvC" sheetId="5" r:id="rId8"/>
+    <sheet name="Graph vs" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="26">
   <si>
     <t>Iteration</t>
   </si>
@@ -81,6 +83,33 @@
   </si>
   <si>
     <t>Player 2</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>good ab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mm ab </t>
+  </si>
+  <si>
+    <t>Min-Max</t>
+  </si>
+  <si>
+    <t>Alpha-Beta</t>
+  </si>
+  <si>
+    <t>Improved Alpha-Beta</t>
+  </si>
+  <si>
+    <t>Depth 7</t>
+  </si>
+  <si>
+    <t>Depth 5</t>
+  </si>
+  <si>
+    <t>Depth 3</t>
   </si>
 </sst>
 </file>
@@ -3599,6 +3628,829 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Average time of finding</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> best possible move</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graph vs'!$C$4:$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Min-Max</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Alpha-Beta</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Improved Alpha-Beta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graph vs'!$D$4:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2927.6987036</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2881.7310616</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.809001599999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1E3B-4E8A-922D-20EF1ABBA6DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="321271408"/>
+        <c:axId val="321272392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="321271408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="321272392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="321272392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="321271408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average time of finding best possible move</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graph vs'!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min-Max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Graph vs'!$D$3:$F$3</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Graph vs'!$D$3:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Depth 7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Depth 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Graph vs'!$D$4:$F$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Graph vs'!$D$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>2927.6987036</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.442805400000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BE15-4DC1-951A-3E58E6FB19A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graph vs'!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Alpha-Beta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Graph vs'!$D$3:$F$3</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Graph vs'!$D$3:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Depth 7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Depth 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Graph vs'!$D$5:$F$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Graph vs'!$D$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>2881.7310616</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.307647800000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BE15-4DC1-951A-3E58E6FB19A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graph vs'!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Improved Alpha-Beta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Graph vs'!$D$3:$F$3</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Graph vs'!$D$3:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Depth 7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Depth 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Graph vs'!$D$6:$F$6</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Graph vs'!$D$6:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>15.809001599999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0564109999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BE15-4DC1-951A-3E58E6FB19A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="315715832"/>
+        <c:axId val="315712224"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="315715832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="315712224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="315712224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="315715832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3879,6 +4731,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -7368,6 +8300,1016 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -7668,6 +9610,83 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BABC0738-C131-47FF-8CB3-FE6D660462C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1585912</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85A9BB81-AC80-40BD-9F67-F49FCC831623}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9838,7 +11857,7 @@
   <dimension ref="A1:AC97"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13480,8 +15499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14169,6 +16188,18 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:G19"/>
   <sheetViews>
@@ -14401,7 +16432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L12"/>
   <sheetViews>
@@ -14741,4 +16772,1055 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:AK26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X25" sqref="X25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2">
+        <v>7</v>
+      </c>
+      <c r="T2">
+        <v>960793</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>5000.0266670000001</v>
+      </c>
+      <c r="W2">
+        <v>57.800708</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z2">
+        <v>5</v>
+      </c>
+      <c r="AA2">
+        <v>19608</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>31.481636000000002</v>
+      </c>
+      <c r="AD2">
+        <v>1.0998760000000001</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG2">
+        <v>3</v>
+      </c>
+      <c r="AH2">
+        <v>400</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0.56245100000000003</v>
+      </c>
+      <c r="AK2">
+        <v>7.3839999999999999E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3">
+        <v>7</v>
+      </c>
+      <c r="T3">
+        <v>960793</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>2795.5227960000002</v>
+      </c>
+      <c r="W3">
+        <v>44.380664000000003</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z3">
+        <v>5</v>
+      </c>
+      <c r="AA3">
+        <v>19608</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>29.222398999999999</v>
+      </c>
+      <c r="AD3">
+        <v>1.267668</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG3">
+        <v>3</v>
+      </c>
+      <c r="AH3">
+        <v>400</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0.877521</v>
+      </c>
+      <c r="AK3">
+        <v>1.8872E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <f>AVERAGE(H4:H8)</f>
+        <v>2927.6987036</v>
+      </c>
+      <c r="E4" s="4">
+        <f>AVERAGE(AC2:AC6)</f>
+        <v>30.442805400000005</v>
+      </c>
+      <c r="F4">
+        <f>AVERAGE(AJ2:AJ6)</f>
+        <v>0.71653979999999995</v>
+      </c>
+      <c r="H4">
+        <v>3543.1468840000002</v>
+      </c>
+      <c r="J4">
+        <v>2822.6344669999999</v>
+      </c>
+      <c r="L4">
+        <v>23.800557000000001</v>
+      </c>
+      <c r="R4" t="s">
+        <v>11</v>
+      </c>
+      <c r="S4">
+        <v>7</v>
+      </c>
+      <c r="T4">
+        <v>960793</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>3186.6092480000002</v>
+      </c>
+      <c r="W4">
+        <v>43.604475000000001</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z4">
+        <v>5</v>
+      </c>
+      <c r="AA4">
+        <v>19608</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>26.500810999999999</v>
+      </c>
+      <c r="AD4">
+        <v>1.2065410000000001</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG4">
+        <v>3</v>
+      </c>
+      <c r="AH4">
+        <v>400</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>1.031774</v>
+      </c>
+      <c r="AK4">
+        <v>1.5179E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <f>D4-AVERAGE(W2:W7)</f>
+        <v>2881.7310616</v>
+      </c>
+      <c r="E5" s="4">
+        <f>E4-AVERAGE(AD2:AD6)</f>
+        <v>29.307647800000005</v>
+      </c>
+      <c r="F5">
+        <f>F4-AVERAGE(AK2:AK6)</f>
+        <v>0.70488899999999999</v>
+      </c>
+      <c r="H5">
+        <v>3186.6092480000002</v>
+      </c>
+      <c r="J5">
+        <v>2945.0570819999998</v>
+      </c>
+      <c r="L5">
+        <v>12.094120999999999</v>
+      </c>
+      <c r="R5" t="s">
+        <v>11</v>
+      </c>
+      <c r="S5">
+        <v>7</v>
+      </c>
+      <c r="T5">
+        <v>960793</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>2409.0902000000001</v>
+      </c>
+      <c r="W5">
+        <v>43.496580000000002</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z5">
+        <v>5</v>
+      </c>
+      <c r="AA5">
+        <v>19608</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>38.515754000000001</v>
+      </c>
+      <c r="AD5">
+        <v>0.93741799999999997</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG5">
+        <v>3</v>
+      </c>
+      <c r="AH5">
+        <v>400</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0.54850200000000005</v>
+      </c>
+      <c r="AK5">
+        <v>9.025E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <f>AVERAGE(L4:L8)</f>
+        <v>15.809001599999998</v>
+      </c>
+      <c r="E6" s="4">
+        <f>AVERAGE(AD20:AD24)</f>
+        <v>2.0564109999999998</v>
+      </c>
+      <c r="F6">
+        <f>AVERAGE(AK20:AK24)</f>
+        <v>9.26342E-2</v>
+      </c>
+      <c r="H6">
+        <v>2409.0902000000001</v>
+      </c>
+      <c r="J6">
+        <v>3188.9681759999999</v>
+      </c>
+      <c r="L6">
+        <v>11.790537</v>
+      </c>
+      <c r="R6" t="s">
+        <v>11</v>
+      </c>
+      <c r="S6">
+        <v>7</v>
+      </c>
+      <c r="T6">
+        <v>960793</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>2677.0127189999998</v>
+      </c>
+      <c r="W6">
+        <v>43.805906999999998</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z6">
+        <v>5</v>
+      </c>
+      <c r="AA6">
+        <v>19608</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>26.493427000000001</v>
+      </c>
+      <c r="AD6">
+        <v>1.164285</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG6">
+        <v>3</v>
+      </c>
+      <c r="AH6">
+        <v>400</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0.56245100000000003</v>
+      </c>
+      <c r="AK6">
+        <v>7.7939999999999997E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="E7" s="4"/>
+      <c r="H7">
+        <v>2677.0127189999998</v>
+      </c>
+      <c r="J7">
+        <v>1670.2505960000001</v>
+      </c>
+      <c r="L7">
+        <v>16.471881</v>
+      </c>
+      <c r="R7" t="s">
+        <v>11</v>
+      </c>
+      <c r="S7">
+        <v>7</v>
+      </c>
+      <c r="T7">
+        <v>960793</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>2822.6344669999999</v>
+      </c>
+      <c r="W7">
+        <v>42.717517999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>2822.6344669999999</v>
+      </c>
+      <c r="J8">
+        <v>2937.3501569999999</v>
+      </c>
+      <c r="L8">
+        <v>14.887912</v>
+      </c>
+    </row>
+    <row r="11" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="R11" t="s">
+        <v>11</v>
+      </c>
+      <c r="S11">
+        <v>7</v>
+      </c>
+      <c r="T11">
+        <v>57414</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>3843.1468840000002</v>
+      </c>
+      <c r="W11">
+        <v>3.4981870000000002</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z11">
+        <v>5</v>
+      </c>
+      <c r="AA11">
+        <v>3620</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>36.802146999999998</v>
+      </c>
+      <c r="AD11">
+        <v>0.68716600000000005</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG11">
+        <v>3</v>
+      </c>
+      <c r="AH11">
+        <v>215</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <v>0.49517</v>
+      </c>
+      <c r="AK11">
+        <v>4.5129999999999997E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="R12" t="s">
+        <v>11</v>
+      </c>
+      <c r="S12">
+        <v>7</v>
+      </c>
+      <c r="T12">
+        <v>57414</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>2945.0570819999998</v>
+      </c>
+      <c r="W12">
+        <v>3.438291</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z12">
+        <v>5</v>
+      </c>
+      <c r="AA12">
+        <v>3620</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>30.629141000000001</v>
+      </c>
+      <c r="AD12">
+        <v>0.28225</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG12">
+        <v>3</v>
+      </c>
+      <c r="AH12">
+        <v>215</v>
+      </c>
+      <c r="AI12">
+        <v>0</v>
+      </c>
+      <c r="AJ12">
+        <v>0.474657</v>
+      </c>
+      <c r="AK12">
+        <v>6.5640000000000004E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="R13" t="s">
+        <v>11</v>
+      </c>
+      <c r="S13">
+        <v>7</v>
+      </c>
+      <c r="T13">
+        <v>57414</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>3188.9681759999999</v>
+      </c>
+      <c r="W13">
+        <v>3.4042400000000002</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z13">
+        <v>5</v>
+      </c>
+      <c r="AA13">
+        <v>3620</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>24.541466</v>
+      </c>
+      <c r="AD13">
+        <v>0.28471200000000002</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG13">
+        <v>3</v>
+      </c>
+      <c r="AH13">
+        <v>215</v>
+      </c>
+      <c r="AI13">
+        <v>0</v>
+      </c>
+      <c r="AJ13">
+        <v>0.721217</v>
+      </c>
+      <c r="AK13">
+        <v>1.1897E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="R14" t="s">
+        <v>11</v>
+      </c>
+      <c r="S14">
+        <v>7</v>
+      </c>
+      <c r="T14">
+        <v>57414</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>1670.2505960000001</v>
+      </c>
+      <c r="W14">
+        <v>3.166296</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z14">
+        <v>5</v>
+      </c>
+      <c r="AA14">
+        <v>3620</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>35.768732</v>
+      </c>
+      <c r="AD14">
+        <v>0.19814999999999999</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG14">
+        <v>3</v>
+      </c>
+      <c r="AH14">
+        <v>215</v>
+      </c>
+      <c r="AI14">
+        <v>0</v>
+      </c>
+      <c r="AJ14">
+        <v>0.52675899999999998</v>
+      </c>
+      <c r="AK14">
+        <v>7.7939999999999997E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="R15" t="s">
+        <v>11</v>
+      </c>
+      <c r="S15">
+        <v>7</v>
+      </c>
+      <c r="T15">
+        <v>57414</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>2937.3501569999999</v>
+      </c>
+      <c r="W15">
+        <v>3.457983</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z15">
+        <v>5</v>
+      </c>
+      <c r="AA15">
+        <v>3620</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>24.725256000000002</v>
+      </c>
+      <c r="AD15">
+        <v>0.30030200000000001</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG15">
+        <v>3</v>
+      </c>
+      <c r="AH15">
+        <v>215</v>
+      </c>
+      <c r="AI15">
+        <v>0</v>
+      </c>
+      <c r="AJ15">
+        <v>0.49640000000000001</v>
+      </c>
+      <c r="AK15">
+        <v>5.744E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="R16" t="s">
+        <v>11</v>
+      </c>
+      <c r="S16">
+        <v>7</v>
+      </c>
+      <c r="T16">
+        <v>57414</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>3215.084175</v>
+      </c>
+      <c r="W16">
+        <v>3.9383840000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="18:37" x14ac:dyDescent="0.25">
+      <c r="R20" t="s">
+        <v>11</v>
+      </c>
+      <c r="S20">
+        <v>7</v>
+      </c>
+      <c r="T20">
+        <v>13167</v>
+      </c>
+      <c r="U20">
+        <v>2540</v>
+      </c>
+      <c r="V20">
+        <v>1.2310000000000001E-3</v>
+      </c>
+      <c r="W20">
+        <v>23.800557000000001</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z20">
+        <v>5</v>
+      </c>
+      <c r="AA20">
+        <v>982</v>
+      </c>
+      <c r="AB20">
+        <v>149</v>
+      </c>
+      <c r="AC20">
+        <v>1.4489970000000001</v>
+      </c>
+      <c r="AD20">
+        <v>5.3566120000000002</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG20">
+        <v>3</v>
+      </c>
+      <c r="AH20">
+        <v>76</v>
+      </c>
+      <c r="AI20">
+        <v>12</v>
+      </c>
+      <c r="AJ20">
+        <v>1.2310000000000001E-3</v>
+      </c>
+      <c r="AK20">
+        <v>8.8613999999999998E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="18:37" x14ac:dyDescent="0.25">
+      <c r="R21" t="s">
+        <v>11</v>
+      </c>
+      <c r="S21">
+        <v>7</v>
+      </c>
+      <c r="T21">
+        <v>13167</v>
+      </c>
+      <c r="U21">
+        <v>2540</v>
+      </c>
+      <c r="V21">
+        <v>1.6410000000000001E-3</v>
+      </c>
+      <c r="W21">
+        <v>12.094120999999999</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z21">
+        <v>5</v>
+      </c>
+      <c r="AA21">
+        <v>982</v>
+      </c>
+      <c r="AB21">
+        <v>149</v>
+      </c>
+      <c r="AC21">
+        <v>2.0509999999999999E-3</v>
+      </c>
+      <c r="AD21">
+        <v>1.4100239999999999</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG21">
+        <v>3</v>
+      </c>
+      <c r="AH21">
+        <v>76</v>
+      </c>
+      <c r="AI21">
+        <v>12</v>
+      </c>
+      <c r="AJ21">
+        <v>1.6410000000000001E-3</v>
+      </c>
+      <c r="AK21">
+        <v>0.106665</v>
+      </c>
+    </row>
+    <row r="22" spans="18:37" x14ac:dyDescent="0.25">
+      <c r="R22" t="s">
+        <v>11</v>
+      </c>
+      <c r="S22">
+        <v>7</v>
+      </c>
+      <c r="T22">
+        <v>13167</v>
+      </c>
+      <c r="U22">
+        <v>2540</v>
+      </c>
+      <c r="V22">
+        <v>1.6410000000000001E-3</v>
+      </c>
+      <c r="W22">
+        <v>11.790537</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z22">
+        <v>5</v>
+      </c>
+      <c r="AA22">
+        <v>982</v>
+      </c>
+      <c r="AB22">
+        <v>149</v>
+      </c>
+      <c r="AC22">
+        <v>2.0509999999999999E-3</v>
+      </c>
+      <c r="AD22">
+        <v>1.5737129999999999</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG22">
+        <v>3</v>
+      </c>
+      <c r="AH22">
+        <v>76</v>
+      </c>
+      <c r="AI22">
+        <v>12</v>
+      </c>
+      <c r="AJ22">
+        <v>1.2310000000000001E-3</v>
+      </c>
+      <c r="AK22">
+        <v>8.0407999999999993E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="18:37" x14ac:dyDescent="0.25">
+      <c r="R23" t="s">
+        <v>11</v>
+      </c>
+      <c r="S23">
+        <v>7</v>
+      </c>
+      <c r="T23">
+        <v>13167</v>
+      </c>
+      <c r="U23">
+        <v>2540</v>
+      </c>
+      <c r="V23">
+        <v>1.23E-3</v>
+      </c>
+      <c r="W23">
+        <v>16.471881</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z23">
+        <v>5</v>
+      </c>
+      <c r="AA23">
+        <v>982</v>
+      </c>
+      <c r="AB23">
+        <v>149</v>
+      </c>
+      <c r="AC23">
+        <v>1.2310000000000001E-3</v>
+      </c>
+      <c r="AD23">
+        <v>0.99116000000000004</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG23">
+        <v>3</v>
+      </c>
+      <c r="AH23">
+        <v>76</v>
+      </c>
+      <c r="AI23">
+        <v>12</v>
+      </c>
+      <c r="AJ23">
+        <v>1.23E-3</v>
+      </c>
+      <c r="AK23">
+        <v>9.2716000000000007E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="18:37" x14ac:dyDescent="0.25">
+      <c r="R24" t="s">
+        <v>11</v>
+      </c>
+      <c r="S24">
+        <v>7</v>
+      </c>
+      <c r="T24">
+        <v>13167</v>
+      </c>
+      <c r="U24">
+        <v>2540</v>
+      </c>
+      <c r="V24">
+        <v>1.2310000000000001E-3</v>
+      </c>
+      <c r="W24">
+        <v>14.887912</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z24">
+        <v>5</v>
+      </c>
+      <c r="AA24">
+        <v>982</v>
+      </c>
+      <c r="AB24">
+        <v>149</v>
+      </c>
+      <c r="AC24">
+        <v>1.2310000000000001E-3</v>
+      </c>
+      <c r="AD24">
+        <v>0.950546</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG24">
+        <v>3</v>
+      </c>
+      <c r="AH24">
+        <v>76</v>
+      </c>
+      <c r="AI24">
+        <v>12</v>
+      </c>
+      <c r="AJ24">
+        <v>1.6410000000000001E-3</v>
+      </c>
+      <c r="AK24">
+        <v>9.4768000000000005E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="18:37" x14ac:dyDescent="0.25">
+      <c r="R25" t="s">
+        <v>11</v>
+      </c>
+      <c r="S25">
+        <v>7</v>
+      </c>
+      <c r="T25">
+        <v>13167</v>
+      </c>
+      <c r="U25">
+        <v>2540</v>
+      </c>
+      <c r="V25">
+        <v>1.2310000000000001E-3</v>
+      </c>
+      <c r="W25">
+        <v>10.918348999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="18:37" x14ac:dyDescent="0.25">
+      <c r="R26" t="s">
+        <v>11</v>
+      </c>
+      <c r="S26">
+        <v>7</v>
+      </c>
+      <c r="T26">
+        <v>13167</v>
+      </c>
+      <c r="U26">
+        <v>2540</v>
+      </c>
+      <c r="V26">
+        <v>2.9947999999999999E-2</v>
+      </c>
+      <c r="W26">
+        <v>10.8363</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>